<commit_message>
TC for URL  added
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20B76F66-2A3F-4A4E-9C54-52431E15CE25}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51A6E593-7998-4037-9244-A4738F559264}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="185">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -240,6 +240,9 @@
     <t>TS_URL_02</t>
   </si>
   <si>
+    <t>TC_URL_03</t>
+  </si>
+  <si>
     <t>FR_URL_04</t>
   </si>
   <si>
@@ -574,6 +577,20 @@
   </si>
   <si>
     <t>TS_NFR_07</t>
+  </si>
+  <si>
+    <t>TC_URL_01</t>
+  </si>
+  <si>
+    <t>TC_URL_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_URL_04
+TC_URL_05
+</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -589,7 +606,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +625,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -621,10 +644,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,7 +1193,7 @@
   <dimension ref="A3:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1202,7 @@
     <col min="2" max="2" width="44.140625" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1209,6 +1242,12 @@
       <c r="D4" t="s">
         <v>61</v>
       </c>
+      <c r="E4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1223,6 +1262,12 @@
       <c r="D5" t="s">
         <v>64</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1237,19 +1282,31 @@
       <c r="D6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" t="s">
         <v>68</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F6" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
-        <v>70</v>
+      <c r="D7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1296,128 +1353,128 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
         <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1425,10 +1482,10 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
@@ -1436,58 +1493,58 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
         <v>101</v>
       </c>
-      <c r="B21" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" t="s">
-        <v>100</v>
-      </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
         <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1495,10 +1552,10 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -1509,10 +1566,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" t="s">
         <v>114</v>
-      </c>
-      <c r="C26" t="s">
-        <v>113</v>
       </c>
       <c r="D26" t="s">
         <v>29</v>
@@ -1520,44 +1577,44 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1565,10 +1622,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D30" t="s">
         <v>34</v>
@@ -1576,58 +1633,58 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" t="s">
         <v>125</v>
       </c>
-      <c r="B31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" t="s">
-        <v>124</v>
-      </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1635,7 +1692,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
@@ -1646,35 +1703,35 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s">
         <v>63</v>
@@ -1683,7 +1740,7 @@
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1691,10 +1748,10 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D39" t="s">
         <v>44</v>
@@ -1705,10 +1762,10 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" t="s">
         <v>147</v>
-      </c>
-      <c r="C40" t="s">
-        <v>146</v>
       </c>
       <c r="D40" t="s">
         <v>48</v>
@@ -1716,58 +1773,58 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C41" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D43" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B44" t="s">
         <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1775,10 +1832,10 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D45" t="s">
         <v>44</v>
@@ -1789,10 +1846,10 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" t="s">
         <v>147</v>
-      </c>
-      <c r="C46" t="s">
-        <v>146</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1800,156 +1857,156 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C47" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D47" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B48" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D48" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C49" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B50" t="s">
         <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B51" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C51" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D51" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C52" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D53" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C54" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D54" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B55" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D56" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B57" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D57" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TC for User reg  added
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51A6E593-7998-4037-9244-A4738F559264}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA03C473-E257-4037-AFAE-4CA1396DB630}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
     <sheet name="RTM_ALL" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="197">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -591,16 +592,58 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Phone number should be validated</t>
+  </si>
+  <si>
+    <t>System should send OTP to valid phone number</t>
+  </si>
+  <si>
+    <t>User should be able to verify OTP</t>
+  </si>
+  <si>
+    <t>FR_REG_05</t>
+  </si>
+  <si>
+    <t>System should handle invalid OTP</t>
+  </si>
+  <si>
+    <t>FR_REG_06</t>
+  </si>
+  <si>
+    <t>System should handle OTP expiry</t>
+  </si>
+  <si>
+    <t>FR_REG_07</t>
+  </si>
+  <si>
+    <t>System should allow OTP resend</t>
+  </si>
+  <si>
+    <t>FR_REG_08</t>
+  </si>
+  <si>
+    <t>FR_REG_09</t>
+  </si>
+  <si>
+    <t>FR_REG_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -673,6 +716,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -962,7 +1009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1190,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE34CF0-8890-43A6-9D70-4DB6854C32E2}">
-  <dimension ref="A3:G57"/>
+  <dimension ref="A3:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,9 +1410,6 @@
       <c r="C11" t="s">
         <v>74</v>
       </c>
-      <c r="D11" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1375,9 +1421,6 @@
       <c r="C12" t="s">
         <v>74</v>
       </c>
-      <c r="D12" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1389,9 +1432,6 @@
       <c r="C13" t="s">
         <v>74</v>
       </c>
-      <c r="D13" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1403,428 +1443,407 @@
       <c r="C14" t="s">
         <v>74</v>
       </c>
-      <c r="D14" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>188</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>186</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>194</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>189</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>191</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>131</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C33" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="D36" t="s">
-        <v>140</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="D37" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>148</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>151</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="B42" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B43" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B44" t="s">
         <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1913,103 +1932,331 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>41</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D51" t="s">
-        <v>163</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>164</v>
+        <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C52" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D52" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="C53" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D53" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C54" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="B55" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="C55" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D55" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B56" t="s">
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D56" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B57" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C57" t="s">
         <v>162</v>
       </c>
       <c r="D57" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" t="s">
+        <v>165</v>
+      </c>
+      <c r="C58" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" t="s">
+        <v>162</v>
+      </c>
+      <c r="D59" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" t="s">
+        <v>171</v>
+      </c>
+      <c r="C60" t="s">
+        <v>162</v>
+      </c>
+      <c r="D60" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B61" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" t="s">
+        <v>162</v>
+      </c>
+      <c r="D61" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>176</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
+        <v>162</v>
+      </c>
+      <c r="D62" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>178</v>
+      </c>
+      <c r="B63" t="s">
+        <v>179</v>
+      </c>
+      <c r="C63" t="s">
+        <v>162</v>
+      </c>
+      <c r="D63" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7495C7C6-8754-40B5-9487-A44731C32792}">
+  <dimension ref="C14:F23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TC for paymnet added
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3360056-3CBB-4E21-844D-D89B6CA9428F}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DD4FF57-DE0A-4B0D-A229-704BFD0CF6A7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="220">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -439,16 +439,10 @@
     <t>FR_PAYMENT_02</t>
   </si>
   <si>
-    <t>Payment success/failure messages</t>
-  </si>
-  <si>
     <t>TS_PAYMENT_02</t>
   </si>
   <si>
     <t>FR_PAYMENT_03</t>
-  </si>
-  <si>
-    <t>Payment info security</t>
   </si>
   <si>
     <t>TS_PAYMENT_03</t>
@@ -636,12 +630,6 @@
     <t>FR_CART_06</t>
   </si>
   <si>
-    <t>User should be able to add product to cart</t>
-  </si>
-  <si>
-    <t>User should be able to update product quantity</t>
-  </si>
-  <si>
     <t>Cart should show correct total price</t>
   </si>
   <si>
@@ -664,6 +652,51 @@
   </si>
   <si>
     <t>Check the payment option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added product details in cart </t>
+  </si>
+  <si>
+    <t>Edit/Delet the product</t>
+  </si>
+  <si>
+    <t>Add product quantity</t>
+  </si>
+  <si>
+    <t>Out of stockproduct should not be added</t>
+  </si>
+  <si>
+    <t>TS_CHECKOUT_06</t>
+  </si>
+  <si>
+    <t>TS_CHECKOUT_07</t>
+  </si>
+  <si>
+    <t>FR_PAYMENT_05</t>
+  </si>
+  <si>
+    <t>FR_PAYMENT_06</t>
+  </si>
+  <si>
+    <t>FR_PAYMENT_07</t>
+  </si>
+  <si>
+    <t>Payment using  Credit/Debit card</t>
+  </si>
+  <si>
+    <t>Payment using UPI</t>
+  </si>
+  <si>
+    <t>Payment using Cash on delivery</t>
+  </si>
+  <si>
+    <t>System should handle payment failure</t>
+  </si>
+  <si>
+    <t>Payment success verfication</t>
+  </si>
+  <si>
+    <t>Secure paymnet</t>
   </si>
 </sst>
 </file>
@@ -1275,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE34CF0-8890-43A6-9D70-4DB6854C32E2}">
-  <dimension ref="A3:G66"/>
+  <dimension ref="A3:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,10 +1361,10 @@
         <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1348,10 +1381,10 @@
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1371,7 +1404,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1388,10 +1421,10 @@
         <v>71</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1494,86 +1527,86 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C15" t="s">
         <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C16" t="s">
         <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
         <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C18" t="s">
         <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C19" t="s">
         <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1721,7 +1754,7 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
         <v>113</v>
@@ -1735,7 +1768,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C32" t="s">
         <v>113</v>
@@ -1749,7 +1782,7 @@
         <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C33" t="s">
         <v>113</v>
@@ -1763,7 +1796,7 @@
         <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C34" t="s">
         <v>113</v>
@@ -1777,7 +1810,7 @@
         <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C35" t="s">
         <v>113</v>
@@ -1788,16 +1821,16 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B36" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C36" t="s">
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1847,7 +1880,7 @@
         <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C40" t="s">
         <v>121</v>
@@ -1861,7 +1894,7 @@
         <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C41" t="s">
         <v>121</v>
@@ -1872,24 +1905,30 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42" t="s">
         <v>203</v>
-      </c>
-      <c r="B42" t="s">
-        <v>207</v>
       </c>
       <c r="C42" t="s">
         <v>121</v>
       </c>
+      <c r="D42" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>200</v>
+      </c>
+      <c r="B43" t="s">
         <v>204</v>
-      </c>
-      <c r="B43" t="s">
-        <v>208</v>
       </c>
       <c r="C43" t="s">
         <v>121</v>
+      </c>
+      <c r="D43" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1911,312 +1950,346 @@
         <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>134</v>
+        <v>214</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="C46" t="s">
         <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>216</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>211</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>217</v>
       </c>
       <c r="C48" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="C49" t="s">
-        <v>142</v>
-      </c>
-      <c r="D49" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>219</v>
       </c>
       <c r="C50" t="s">
-        <v>142</v>
-      </c>
-      <c r="D50" t="s">
-        <v>146</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>152</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D53" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D54" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C55" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D55" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
-        <v>145</v>
+        <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D56" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>152</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D59" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B60" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="D60" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B61" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="D61" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s">
-        <v>163</v>
+        <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="D62" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C63" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D64" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>161</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D65" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" t="s">
+        <v>155</v>
+      </c>
+      <c r="D66" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>166</v>
+      </c>
+      <c r="B67" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>169</v>
+      </c>
+      <c r="B68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" t="s">
+        <v>172</v>
+      </c>
+      <c r="C69" t="s">
+        <v>155</v>
+      </c>
+      <c r="D69" t="s">
         <v>173</v>
-      </c>
-      <c r="B66" t="s">
-        <v>174</v>
-      </c>
-      <c r="C66" t="s">
-        <v>157</v>
-      </c>
-      <c r="D66" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2294,10 +2367,10 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E18" t="s">
         <v>74</v>
@@ -2305,10 +2378,10 @@
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E19" t="s">
         <v>74</v>
@@ -2316,10 +2389,10 @@
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E20" t="s">
         <v>74</v>
@@ -2327,10 +2400,10 @@
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D21" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E21" t="s">
         <v>74</v>
@@ -2338,10 +2411,10 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D22" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E22" t="s">
         <v>74</v>
@@ -2349,10 +2422,10 @@
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E23" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
TC for Order tracking and cancelltion updated
</commit_message>
<xml_diff>
--- a/RTM_All_Modules.xlsx
+++ b/RTM_All_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88952B13-BD3B-4020-A01D-F1506F8AFD5C}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="8_{4EDD0A8C-986B-47C9-B440-4E61EB727780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9865239-5809-4789-9EC7-861CCC179F71}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="245">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -706,6 +706,72 @@
   </si>
   <si>
     <t>Confirmation email/SMS should be sent</t>
+  </si>
+  <si>
+    <t>TS_ORDER_07</t>
+  </si>
+  <si>
+    <t>TS_PAYMENT_05</t>
+  </si>
+  <si>
+    <t>TS_PAYMENT_06</t>
+  </si>
+  <si>
+    <t>TS_PAYMENT_07</t>
+  </si>
+  <si>
+    <t>FR_OT_01</t>
+  </si>
+  <si>
+    <t>FR_OT_02</t>
+  </si>
+  <si>
+    <t>FR_OT_03</t>
+  </si>
+  <si>
+    <t>FR_OT_04</t>
+  </si>
+  <si>
+    <t>FR_OT_05</t>
+  </si>
+  <si>
+    <t>FR_OT_06</t>
+  </si>
+  <si>
+    <t>View Order Status</t>
+  </si>
+  <si>
+    <t>Order Tracking update</t>
+  </si>
+  <si>
+    <t>Cancel the Order before shipment</t>
+  </si>
+  <si>
+    <t>System should not allow cancellation after shipment</t>
+  </si>
+  <si>
+    <t>Cancellation confirmation message should be displayed</t>
+  </si>
+  <si>
+    <t>Order Tracking &amp; Cancellation</t>
+  </si>
+  <si>
+    <t>TS_OT_01</t>
+  </si>
+  <si>
+    <t>TS_OT_04</t>
+  </si>
+  <si>
+    <t>TS_OT_02</t>
+  </si>
+  <si>
+    <t>TS_OT_03</t>
+  </si>
+  <si>
+    <t>TS_OT_05</t>
+  </si>
+  <si>
+    <t>TS_OT_06</t>
   </si>
 </sst>
 </file>
@@ -1317,17 +1383,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE34CF0-8890-43A6-9D70-4DB6854C32E2}">
-  <dimension ref="A3:G64"/>
+  <dimension ref="A3:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:E54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
@@ -2006,6 +2072,9 @@
       <c r="C48" t="s">
         <v>38</v>
       </c>
+      <c r="D48" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -2017,6 +2086,9 @@
       <c r="C49" t="s">
         <v>38</v>
       </c>
+      <c r="D49" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -2028,6 +2100,9 @@
       <c r="C50" t="s">
         <v>38</v>
       </c>
+      <c r="D50" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -2123,102 +2198,189 @@
       <c r="C57" t="s">
         <v>140</v>
       </c>
+      <c r="D57" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>233</v>
       </c>
       <c r="C58" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="D58" t="s">
-        <v>153</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>228</v>
       </c>
       <c r="B59" t="s">
-        <v>155</v>
+        <v>234</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="D59" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>157</v>
+        <v>229</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="C60" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="D60" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>160</v>
+        <v>230</v>
       </c>
       <c r="B61" t="s">
-        <v>161</v>
+        <v>236</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="D61" t="s">
-        <v>162</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>163</v>
+        <v>231</v>
       </c>
       <c r="B62" t="s">
-        <v>164</v>
+        <v>237</v>
       </c>
       <c r="C62" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="D62" t="s">
-        <v>165</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>232</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>237</v>
       </c>
       <c r="C63" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="C64" t="s">
         <v>152</v>
       </c>
       <c r="D64" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65" t="s">
+        <v>152</v>
+      </c>
+      <c r="D65" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67" t="s">
+        <v>161</v>
+      </c>
+      <c r="C67" t="s">
+        <v>152</v>
+      </c>
+      <c r="D67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" t="s">
+        <v>152</v>
+      </c>
+      <c r="D68" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>166</v>
+      </c>
+      <c r="B69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" t="s">
+        <v>152</v>
+      </c>
+      <c r="D69" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>168</v>
+      </c>
+      <c r="B70" t="s">
+        <v>169</v>
+      </c>
+      <c r="C70" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>